<commit_message>
Changed Cases.xlsx and Check.xlsx
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\Testing\Diplom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61295F2A-06E0-4547-8C9D-76177B22E5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9157595F-0ABA-40FB-B878-11053394CAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10500" yWindow="765" windowWidth="15390" windowHeight="15630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10785" yWindow="0" windowWidth="17325" windowHeight="15630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$D$189</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$D$190</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="212">
   <si>
     <t>Группа проверок/модуль</t>
   </si>
@@ -1989,6 +1989,9 @@
       </rPr>
       <t>Back</t>
     </r>
+  </si>
+  <si>
+    <t>Изменение ориентации экрана при нахождении на странице авторизации</t>
   </si>
 </sst>
 </file>
@@ -2280,41 +2283,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2323,6 +2314,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2648,10 +2651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E189"/>
+  <dimension ref="A1:E190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="C180" sqref="C180:C188"/>
+    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
+      <selection activeCell="B162" sqref="B162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2678,15 +2681,15 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="30" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -2700,7 +2703,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="10" t="s">
         <v>11</v>
       </c>
@@ -2712,7 +2715,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="10" t="s">
         <v>12</v>
       </c>
@@ -2724,7 +2727,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="10" t="s">
         <v>15</v>
       </c>
@@ -2736,7 +2739,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="10" t="s">
         <v>13</v>
       </c>
@@ -2748,7 +2751,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="10" t="s">
         <v>14</v>
       </c>
@@ -2774,7 +2777,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="30" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -2788,7 +2791,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="10" t="s">
         <v>17</v>
       </c>
@@ -2800,7 +2803,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="10" t="s">
         <v>195</v>
       </c>
@@ -2812,7 +2815,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="10" t="s">
         <v>136</v>
       </c>
@@ -2824,7 +2827,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="10" t="s">
         <v>18</v>
       </c>
@@ -2836,7 +2839,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
+      <c r="A15" s="30"/>
       <c r="B15" s="10" t="s">
         <v>196</v>
       </c>
@@ -2848,7 +2851,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="10" t="s">
         <v>137</v>
       </c>
@@ -2860,7 +2863,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="10" t="s">
         <v>197</v>
       </c>
@@ -2872,7 +2875,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="10" t="s">
         <v>22</v>
       </c>
@@ -2884,7 +2887,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="10" t="s">
         <v>19</v>
       </c>
@@ -2896,7 +2899,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="10" t="s">
         <v>194</v>
       </c>
@@ -2908,7 +2911,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="10" t="s">
         <v>145</v>
       </c>
@@ -2920,7 +2923,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="10" t="s">
         <v>198</v>
       </c>
@@ -2932,12 +2935,12 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
@@ -2954,12 +2957,12 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
@@ -3168,7 +3171,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="20" t="s">
         <v>36</v>
       </c>
       <c r="B43" s="10" t="s">
@@ -3182,7 +3185,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="26"/>
+      <c r="A44" s="21"/>
       <c r="B44" s="10" t="s">
         <v>39</v>
       </c>
@@ -3194,7 +3197,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="26"/>
+      <c r="A45" s="21"/>
       <c r="B45" s="10" t="s">
         <v>147</v>
       </c>
@@ -3206,7 +3209,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="26"/>
+      <c r="A46" s="21"/>
       <c r="B46" s="10" t="s">
         <v>149</v>
       </c>
@@ -3218,7 +3221,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="26"/>
+      <c r="A47" s="21"/>
       <c r="B47" s="10" t="s">
         <v>199</v>
       </c>
@@ -3230,7 +3233,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="26"/>
+      <c r="A48" s="21"/>
       <c r="B48" s="10" t="s">
         <v>89</v>
       </c>
@@ -3242,7 +3245,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="26"/>
+      <c r="A49" s="21"/>
       <c r="B49" s="10" t="s">
         <v>40</v>
       </c>
@@ -3254,7 +3257,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="26"/>
+      <c r="A50" s="21"/>
       <c r="B50" s="10" t="s">
         <v>41</v>
       </c>
@@ -3266,7 +3269,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="26"/>
+      <c r="A51" s="21"/>
       <c r="B51" s="10" t="s">
         <v>42</v>
       </c>
@@ -3278,7 +3281,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="26"/>
+      <c r="A52" s="21"/>
       <c r="B52" s="10" t="s">
         <v>44</v>
       </c>
@@ -3290,7 +3293,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="26"/>
+      <c r="A53" s="21"/>
       <c r="B53" s="10" t="s">
         <v>37</v>
       </c>
@@ -3302,7 +3305,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="26"/>
+      <c r="A54" s="21"/>
       <c r="B54" s="10" t="s">
         <v>46</v>
       </c>
@@ -3314,7 +3317,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="26"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="10" t="s">
         <v>43</v>
       </c>
@@ -3326,7 +3329,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="26"/>
+      <c r="A56" s="21"/>
       <c r="B56" s="10" t="s">
         <v>45</v>
       </c>
@@ -3338,7 +3341,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="26"/>
+      <c r="A57" s="21"/>
       <c r="B57" s="10" t="s">
         <v>47</v>
       </c>
@@ -3350,7 +3353,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="26"/>
+      <c r="A58" s="21"/>
       <c r="B58" s="10" t="s">
         <v>48</v>
       </c>
@@ -3362,7 +3365,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="26"/>
+      <c r="A59" s="21"/>
       <c r="B59" s="10" t="s">
         <v>50</v>
       </c>
@@ -3374,7 +3377,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="26"/>
+      <c r="A60" s="21"/>
       <c r="B60" s="10" t="s">
         <v>51</v>
       </c>
@@ -3386,7 +3389,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="26"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="10" t="s">
         <v>52</v>
       </c>
@@ -3398,7 +3401,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="23"/>
+      <c r="A62" s="22"/>
       <c r="B62" s="10" t="s">
         <v>53</v>
       </c>
@@ -3712,15 +3715,15 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="21" t="s">
+      <c r="A88" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="B88" s="21"/>
-      <c r="C88" s="21"/>
-      <c r="D88" s="21"/>
+      <c r="B88" s="23"/>
+      <c r="C88" s="23"/>
+      <c r="D88" s="23"/>
     </row>
     <row r="89" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="22" t="s">
+      <c r="A89" s="20" t="s">
         <v>64</v>
       </c>
       <c r="B89" s="10" t="s">
@@ -3733,8 +3736,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="23"/>
+    <row r="90" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="22"/>
       <c r="B90" s="10" t="s">
         <v>80</v>
       </c>
@@ -3746,7 +3749,7 @@
       </c>
     </row>
     <row r="91" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="30" t="s">
+      <c r="A91" s="26" t="s">
         <v>65</v>
       </c>
       <c r="B91" s="10" t="s">
@@ -3760,7 +3763,7 @@
       </c>
     </row>
     <row r="92" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="31"/>
+      <c r="A92" s="27"/>
       <c r="B92" s="10" t="s">
         <v>67</v>
       </c>
@@ -3772,7 +3775,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="31"/>
+      <c r="A93" s="27"/>
       <c r="B93" s="10" t="s">
         <v>66</v>
       </c>
@@ -3784,7 +3787,7 @@
       </c>
     </row>
     <row r="94" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A94" s="31"/>
+      <c r="A94" s="27"/>
       <c r="B94" s="10" t="s">
         <v>167</v>
       </c>
@@ -3796,7 +3799,7 @@
       </c>
     </row>
     <row r="95" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A95" s="31"/>
+      <c r="A95" s="27"/>
       <c r="B95" s="10" t="s">
         <v>168</v>
       </c>
@@ -3808,7 +3811,7 @@
       </c>
     </row>
     <row r="96" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A96" s="31"/>
+      <c r="A96" s="27"/>
       <c r="B96" s="10" t="s">
         <v>169</v>
       </c>
@@ -3820,7 +3823,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="31"/>
+      <c r="A97" s="27"/>
       <c r="B97" s="10" t="s">
         <v>170</v>
       </c>
@@ -3832,7 +3835,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="32"/>
+      <c r="A98" s="28"/>
       <c r="B98" s="10" t="s">
         <v>68</v>
       </c>
@@ -3966,7 +3969,7 @@
       </c>
     </row>
     <row r="109" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="22" t="s">
+      <c r="A109" s="20" t="s">
         <v>106</v>
       </c>
       <c r="B109" s="10" t="s">
@@ -3980,7 +3983,7 @@
       </c>
     </row>
     <row r="110" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A110" s="26"/>
+      <c r="A110" s="21"/>
       <c r="B110" s="10" t="s">
         <v>70</v>
       </c>
@@ -3992,7 +3995,7 @@
       </c>
     </row>
     <row r="111" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A111" s="26"/>
+      <c r="A111" s="21"/>
       <c r="B111" s="10" t="s">
         <v>71</v>
       </c>
@@ -4004,7 +4007,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A112" s="26"/>
+      <c r="A112" s="21"/>
       <c r="B112" s="10" t="s">
         <v>74</v>
       </c>
@@ -4016,7 +4019,7 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A113" s="26"/>
+      <c r="A113" s="21"/>
       <c r="B113" s="10" t="s">
         <v>75</v>
       </c>
@@ -4028,7 +4031,7 @@
       </c>
     </row>
     <row r="114" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A114" s="26"/>
+      <c r="A114" s="21"/>
       <c r="B114" s="10" t="s">
         <v>76</v>
       </c>
@@ -4040,7 +4043,7 @@
       </c>
     </row>
     <row r="115" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A115" s="26"/>
+      <c r="A115" s="21"/>
       <c r="B115" s="10" t="s">
         <v>72</v>
       </c>
@@ -4052,7 +4055,7 @@
       </c>
     </row>
     <row r="116" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A116" s="26"/>
+      <c r="A116" s="21"/>
       <c r="B116" s="10" t="s">
         <v>73</v>
       </c>
@@ -4064,7 +4067,7 @@
       </c>
     </row>
     <row r="117" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A117" s="26"/>
+      <c r="A117" s="21"/>
       <c r="B117" s="10" t="s">
         <v>77</v>
       </c>
@@ -4076,7 +4079,7 @@
       </c>
     </row>
     <row r="118" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A118" s="26"/>
+      <c r="A118" s="21"/>
       <c r="B118" s="10" t="s">
         <v>78</v>
       </c>
@@ -4088,7 +4091,7 @@
       </c>
     </row>
     <row r="119" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A119" s="26"/>
+      <c r="A119" s="21"/>
       <c r="B119" s="10" t="s">
         <v>205</v>
       </c>
@@ -4100,7 +4103,7 @@
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="23"/>
+      <c r="A120" s="22"/>
       <c r="B120" s="10" t="s">
         <v>79</v>
       </c>
@@ -4112,7 +4115,7 @@
       </c>
     </row>
     <row r="121" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="22" t="s">
+      <c r="A121" s="20" t="s">
         <v>107</v>
       </c>
       <c r="B121" s="10" t="s">
@@ -4126,7 +4129,7 @@
       </c>
     </row>
     <row r="122" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="26"/>
+      <c r="A122" s="21"/>
       <c r="B122" s="10" t="s">
         <v>180</v>
       </c>
@@ -4138,7 +4141,7 @@
       </c>
     </row>
     <row r="123" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="26"/>
+      <c r="A123" s="21"/>
       <c r="B123" s="10" t="s">
         <v>183</v>
       </c>
@@ -4150,7 +4153,7 @@
       </c>
     </row>
     <row r="124" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="26"/>
+      <c r="A124" s="21"/>
       <c r="B124" s="10" t="s">
         <v>181</v>
       </c>
@@ -4162,7 +4165,7 @@
       </c>
     </row>
     <row r="125" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="26"/>
+      <c r="A125" s="21"/>
       <c r="B125" s="10" t="s">
         <v>184</v>
       </c>
@@ -4174,7 +4177,7 @@
       </c>
     </row>
     <row r="126" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A126" s="26"/>
+      <c r="A126" s="21"/>
       <c r="B126" s="10" t="s">
         <v>81</v>
       </c>
@@ -4186,7 +4189,7 @@
       </c>
     </row>
     <row r="127" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A127" s="23"/>
+      <c r="A127" s="22"/>
       <c r="B127" s="10" t="s">
         <v>206</v>
       </c>
@@ -4198,12 +4201,12 @@
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="21" t="s">
+      <c r="A128" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="B128" s="21"/>
-      <c r="C128" s="21"/>
-      <c r="D128" s="21"/>
+      <c r="B128" s="23"/>
+      <c r="C128" s="23"/>
+      <c r="D128" s="23"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="15" t="s">
@@ -4220,15 +4223,15 @@
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" s="27" t="s">
+      <c r="A130" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="B130" s="28"/>
-      <c r="C130" s="28"/>
-      <c r="D130" s="28"/>
+      <c r="B130" s="25"/>
+      <c r="C130" s="25"/>
+      <c r="D130" s="25"/>
     </row>
     <row r="131" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="22" t="s">
+      <c r="A131" s="20" t="s">
         <v>88</v>
       </c>
       <c r="B131" s="10" t="s">
@@ -4242,7 +4245,7 @@
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" s="26"/>
+      <c r="A132" s="21"/>
       <c r="B132" s="10" t="s">
         <v>116</v>
       </c>
@@ -4254,7 +4257,7 @@
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" s="26"/>
+      <c r="A133" s="21"/>
       <c r="B133" s="10" t="s">
         <v>86</v>
       </c>
@@ -4266,7 +4269,7 @@
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" s="23"/>
+      <c r="A134" s="22"/>
       <c r="B134" s="10" t="s">
         <v>87</v>
       </c>
@@ -4278,15 +4281,15 @@
       </c>
     </row>
     <row r="135" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A135" s="25" t="s">
+      <c r="A135" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="B135" s="25"/>
-      <c r="C135" s="25"/>
-      <c r="D135" s="25"/>
+      <c r="B135" s="19"/>
+      <c r="C135" s="19"/>
+      <c r="D135" s="19"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" s="18" t="s">
+      <c r="A136" s="30" t="s">
         <v>4</v>
       </c>
       <c r="B136" s="10" t="s">
@@ -4303,7 +4306,7 @@
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" s="18"/>
+      <c r="A137" s="30"/>
       <c r="B137" s="10" t="s">
         <v>6</v>
       </c>
@@ -4318,7 +4321,7 @@
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A138" s="18" t="s">
+      <c r="A138" s="30" t="s">
         <v>94</v>
       </c>
       <c r="B138" s="10" t="s">
@@ -4332,7 +4335,7 @@
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" s="18"/>
+      <c r="A139" s="30"/>
       <c r="B139" s="10" t="s">
         <v>185</v>
       </c>
@@ -4344,7 +4347,7 @@
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" s="18"/>
+      <c r="A140" s="30"/>
       <c r="B140" s="10" t="s">
         <v>96</v>
       </c>
@@ -4356,7 +4359,7 @@
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" s="18"/>
+      <c r="A141" s="30"/>
       <c r="B141" s="10" t="s">
         <v>186</v>
       </c>
@@ -4368,7 +4371,7 @@
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A142" s="18"/>
+      <c r="A142" s="30"/>
       <c r="B142" s="10" t="s">
         <v>97</v>
       </c>
@@ -4380,7 +4383,7 @@
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A143" s="18" t="s">
+      <c r="A143" s="30" t="s">
         <v>98</v>
       </c>
       <c r="B143" s="10" t="s">
@@ -4394,7 +4397,7 @@
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A144" s="18"/>
+      <c r="A144" s="30"/>
       <c r="B144" s="10" t="s">
         <v>100</v>
       </c>
@@ -4406,59 +4409,59 @@
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="18"/>
+      <c r="A145" s="30"/>
       <c r="B145" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C145" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D145" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="30"/>
+      <c r="B146" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C145" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D145" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="18"/>
-      <c r="B146" s="10" t="s">
+      <c r="C146" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D146" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="30"/>
+      <c r="B147" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="C146" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D146" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="18"/>
-      <c r="B147" s="10" t="s">
+      <c r="C147" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D147" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="30"/>
+      <c r="B148" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="C147" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D147" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="18" t="s">
+      <c r="C148" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D148" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="B148" s="10" t="s">
+      <c r="B149" s="10" t="s">
         <v>103</v>
-      </c>
-      <c r="C148" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D148" s="13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="18"/>
-      <c r="B149" s="10" t="s">
-        <v>104</v>
       </c>
       <c r="C149" s="4" t="s">
         <v>7</v>
@@ -4468,9 +4471,9 @@
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="18"/>
+      <c r="A150" s="30"/>
       <c r="B150" s="10" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C150" s="4" t="s">
         <v>7</v>
@@ -4480,69 +4483,69 @@
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="18"/>
+      <c r="A151" s="30"/>
       <c r="B151" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C151" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D151" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="30"/>
+      <c r="B152" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="C151" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D151" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="18"/>
-      <c r="B152" s="10" t="s">
+      <c r="C152" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D152" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="30"/>
+      <c r="B153" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C152" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D152" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="18"/>
-      <c r="B153" s="10" t="s">
+      <c r="C153" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D153" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="30"/>
+      <c r="B154" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="C153" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D153" s="13" t="s">
+      <c r="C154" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D154" s="13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="18"/>
-      <c r="B154" s="10" t="s">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="30"/>
+      <c r="B155" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C154" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D154" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="18"/>
-      <c r="B155" s="10" t="s">
+      <c r="C155" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D155" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="30"/>
+      <c r="B156" s="10" t="s">
         <v>110</v>
-      </c>
-      <c r="C155" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D155" s="13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="18"/>
-      <c r="B156" s="10" t="s">
-        <v>112</v>
       </c>
       <c r="C156" s="4" t="s">
         <v>7</v>
@@ -4552,45 +4555,45 @@
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="18"/>
+      <c r="A157" s="30"/>
       <c r="B157" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C157" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D157" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="30"/>
+      <c r="B158" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="C157" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D157" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="18"/>
-      <c r="B158" s="10" t="s">
+      <c r="C158" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D158" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="30"/>
+      <c r="B159" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C158" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D158" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="18"/>
-      <c r="B159" s="10" t="s">
+      <c r="C159" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D159" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="30"/>
+      <c r="B160" s="10" t="s">
         <v>114</v>
-      </c>
-      <c r="C159" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D159" s="13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="18"/>
-      <c r="B160" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="C160" s="4" t="s">
         <v>7</v>
@@ -4600,9 +4603,9 @@
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="18"/>
+      <c r="A161" s="30"/>
       <c r="B161" s="10" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C161" s="4" t="s">
         <v>7</v>
@@ -4612,35 +4615,35 @@
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="18"/>
+      <c r="A162" s="30"/>
       <c r="B162" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C162" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D162" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="30"/>
+      <c r="B163" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C162" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D162" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="19" t="s">
+      <c r="C163" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D163" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="31" t="s">
         <v>188</v>
       </c>
-      <c r="B163" s="10" t="s">
+      <c r="B164" s="10" t="s">
         <v>189</v>
-      </c>
-      <c r="C163" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D163" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="33"/>
-      <c r="B164" s="10" t="s">
-        <v>190</v>
       </c>
       <c r="C164" s="4" t="s">
         <v>7</v>
@@ -4652,205 +4655,205 @@
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="33"/>
       <c r="B165" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="C165" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D165" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="33"/>
+      <c r="B166" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="C165" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D165" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="20"/>
-      <c r="B166" s="10" t="s">
+      <c r="C166" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D166" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="32"/>
+      <c r="B167" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="C166" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D166" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="18" t="s">
+      <c r="C167" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D167" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="B167" s="10" t="s">
+      <c r="B168" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C167" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D167" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="18"/>
-      <c r="B168" s="10" t="s">
+      <c r="C168" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D168" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="30"/>
+      <c r="B169" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C168" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D168" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="18"/>
-      <c r="B169" s="10" t="s">
+      <c r="C169" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D169" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="30"/>
+      <c r="B170" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C169" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D169" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="18"/>
-      <c r="B170" s="10" t="s">
+      <c r="C170" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D170" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="30"/>
+      <c r="B171" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="C170" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D170" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="18"/>
-      <c r="B171" s="10" t="s">
+      <c r="C171" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D171" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="30"/>
+      <c r="B172" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="C171" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D171" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="18"/>
-      <c r="B172" s="10" t="s">
+      <c r="C172" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D172" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="30"/>
+      <c r="B173" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="C172" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D172" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="18"/>
-      <c r="B173" s="10" t="s">
+      <c r="C173" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D173" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="30"/>
+      <c r="B174" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="C173" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D173" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="18"/>
-      <c r="B174" s="10" t="s">
+      <c r="C174" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D174" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="30"/>
+      <c r="B175" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="C174" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D174" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="18"/>
-      <c r="B175" s="10" t="s">
+      <c r="C175" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D175" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="30"/>
+      <c r="B176" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C175" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D175" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="18"/>
-      <c r="B176" s="10" t="s">
+      <c r="C176" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D176" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="30"/>
+      <c r="B177" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C176" s="4" t="s">
+      <c r="C177" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D176" s="13" t="s">
+      <c r="D177" s="13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="18"/>
-      <c r="B177" s="10" t="s">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="30"/>
+      <c r="B178" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C177" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D177" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="19" t="s">
+      <c r="C178" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D178" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="B178" s="10" t="s">
+      <c r="B179" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C178" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D178" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="20"/>
-      <c r="B179" s="10" t="s">
+      <c r="C179" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D179" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="32"/>
+      <c r="B180" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="C179" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D179" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="18" t="s">
+      <c r="C180" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D180" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="B180" s="10" t="s">
+      <c r="B181" s="10" t="s">
         <v>129</v>
-      </c>
-      <c r="C180" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D180" s="13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A181" s="18"/>
-      <c r="B181" s="10" t="s">
-        <v>193</v>
       </c>
       <c r="C181" s="17" t="s">
         <v>35</v>
@@ -4859,10 +4862,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="18"/>
+    <row r="182" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A182" s="30"/>
       <c r="B182" s="10" t="s">
-        <v>163</v>
+        <v>193</v>
       </c>
       <c r="C182" s="17" t="s">
         <v>35</v>
@@ -4872,9 +4875,9 @@
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="18"/>
+      <c r="A183" s="30"/>
       <c r="B183" s="10" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
       <c r="C183" s="17" t="s">
         <v>35</v>
@@ -4884,9 +4887,9 @@
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="18"/>
+      <c r="A184" s="30"/>
       <c r="B184" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C184" s="17" t="s">
         <v>35</v>
@@ -4896,9 +4899,9 @@
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="18"/>
+      <c r="A185" s="30"/>
       <c r="B185" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C185" s="17" t="s">
         <v>35</v>
@@ -4908,9 +4911,9 @@
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="18"/>
+      <c r="A186" s="30"/>
       <c r="B186" s="10" t="s">
-        <v>164</v>
+        <v>128</v>
       </c>
       <c r="C186" s="17" t="s">
         <v>35</v>
@@ -4920,9 +4923,9 @@
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="18"/>
+      <c r="A187" s="30"/>
       <c r="B187" s="10" t="s">
-        <v>130</v>
+        <v>164</v>
       </c>
       <c r="C187" s="17" t="s">
         <v>35</v>
@@ -4932,9 +4935,9 @@
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="18"/>
+      <c r="A188" s="30"/>
       <c r="B188" s="10" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="C188" s="17" t="s">
         <v>35</v>
@@ -4943,10 +4946,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A189" s="18"/>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="30"/>
       <c r="B189" s="10" t="s">
-        <v>210</v>
+        <v>148</v>
       </c>
       <c r="C189" s="17" t="s">
         <v>35</v>
@@ -4955,9 +4958,32 @@
         <v>49</v>
       </c>
     </row>
+    <row r="190" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A190" s="30"/>
+      <c r="B190" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="C190" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D190" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D189" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D190" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="26">
+    <mergeCell ref="A181:A190"/>
+    <mergeCell ref="A179:A180"/>
+    <mergeCell ref="A149:A163"/>
+    <mergeCell ref="A168:A178"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A88:D88"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="A136:A137"/>
+    <mergeCell ref="A138:A142"/>
+    <mergeCell ref="A143:A148"/>
+    <mergeCell ref="A164:A167"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A135:D135"/>
     <mergeCell ref="A121:A127"/>
@@ -4973,17 +4999,6 @@
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="A10:A22"/>
     <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A180:A189"/>
-    <mergeCell ref="A178:A179"/>
-    <mergeCell ref="A148:A162"/>
-    <mergeCell ref="A167:A177"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A88:D88"/>
-    <mergeCell ref="A89:A90"/>
-    <mergeCell ref="A136:A137"/>
-    <mergeCell ref="A138:A142"/>
-    <mergeCell ref="A143:A147"/>
-    <mergeCell ref="A163:A166"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>